<commit_message>
added choreography for objects and smoke machine
</commit_message>
<xml_diff>
--- a/Choreography.xlsx
+++ b/Choreography.xlsx
@@ -8,14 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc279616e9bf515a/Desktop/Robert/Uni/Fundamentals of Programming/Assignment V2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{872808D0-E74D-4280-8616-FE908870EFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9028684F-FBEA-482F-B568-AAB50E69B2BE}"/>
+  <xr:revisionPtr revIDLastSave="326" documentId="8_{872808D0-E74D-4280-8616-FE908870EFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51037147-5BD4-493D-B371-40C275FB3597}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="2316" windowWidth="17280" windowHeight="8880" xr2:uid="{CA1F9D46-EE91-46A4-B57B-4EC92E55F95A}"/>
+    <workbookView xWindow="-28920" yWindow="-6795" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{CA1F9D46-EE91-46A4-B57B-4EC92E55F95A}"/>
   </bookViews>
   <sheets>
     <sheet name="init" sheetId="1" r:id="rId1"/>
     <sheet name="Light1" sheetId="2" r:id="rId2"/>
     <sheet name="Light2" sheetId="3" r:id="rId3"/>
+    <sheet name="Light3" sheetId="9" r:id="rId4"/>
+    <sheet name="Light4" sheetId="8" r:id="rId5"/>
+    <sheet name="machine1" sheetId="4" r:id="rId6"/>
+    <sheet name="machine2" sheetId="7" r:id="rId7"/>
+    <sheet name="guitar" sheetId="6" r:id="rId8"/>
+    <sheet name="Key info" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="62">
   <si>
     <t>Type</t>
   </si>
@@ -91,9 +97,6 @@
     <t>Speed</t>
   </si>
   <si>
-    <t>Position(Co-ordinate)</t>
-  </si>
-  <si>
     <t>Light1</t>
   </si>
   <si>
@@ -149,6 +152,84 @@
   </si>
   <si>
     <t>Loop To</t>
+  </si>
+  <si>
+    <t>machine1</t>
+  </si>
+  <si>
+    <t>Vertical Position</t>
+  </si>
+  <si>
+    <t>Must Have sheet named "init"</t>
+  </si>
+  <si>
+    <t>In init stage setup must be in line 3</t>
+  </si>
+  <si>
+    <t>Instructions:</t>
+  </si>
+  <si>
+    <t>Will arrive at the destination at the specified time</t>
+  </si>
+  <si>
+    <t>Will go back to a specified row index(starting at 0 from row 2 in excel)</t>
+  </si>
+  <si>
+    <t>Hold</t>
+  </si>
+  <si>
+    <t>Does Nothing until end time</t>
+  </si>
+  <si>
+    <t>Name of thing must be the same as corresponding sheet name</t>
+  </si>
+  <si>
+    <t>Never Moves again</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Stops entire program</t>
+  </si>
+  <si>
+    <t>Column order matters</t>
+  </si>
+  <si>
+    <t>backdrop.png</t>
+  </si>
+  <si>
+    <t>guitar</t>
+  </si>
+  <si>
+    <t>guitar.png</t>
+  </si>
+  <si>
+    <t>Rotation</t>
+  </si>
+  <si>
+    <t>machine2</t>
+  </si>
+  <si>
+    <t>Light3</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>Light4</t>
+  </si>
+  <si>
+    <t>magenta</t>
+  </si>
+  <si>
+    <t>cyan</t>
+  </si>
+  <si>
+    <t>yellow</t>
   </si>
 </sst>
 </file>
@@ -504,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E3453A-179F-4C57-94EA-DC41270CAC58}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,25 +598,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>30</v>
-      </c>
-      <c r="H1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -549,12 +630,12 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>512</v>
@@ -563,7 +644,10 @@
         <v>288</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0.1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -594,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>256</v>
@@ -612,7 +696,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -620,7 +704,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>256</v>
@@ -629,7 +713,7 @@
         <v>-45</v>
       </c>
       <c r="E7">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F7">
         <v>30</v>
@@ -638,45 +722,168 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8">
+        <v>150</v>
+      </c>
+      <c r="D8">
+        <v>-30</v>
+      </c>
+      <c r="E8">
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
       <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9">
+        <v>500</v>
+      </c>
+      <c r="D9">
+        <v>-100</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>45</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
+      <c r="E12">
         <v>4</v>
+      </c>
+      <c r="F12">
+        <v>45</v>
+      </c>
+      <c r="G12">
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13">
+        <v>500</v>
+      </c>
+      <c r="D13">
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>135</v>
+      </c>
+      <c r="G13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16">
+        <v>400</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -689,7 +896,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,10 +906,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
       </c>
       <c r="C1" t="s">
         <v>15</v>
@@ -720,12 +927,12 @@
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -740,18 +947,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB9F836-1785-4051-A1F8-E06C1617609E}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
       </c>
       <c r="C1" t="s">
         <v>15</v>
@@ -769,12 +976,12 @@
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -783,13 +990,13 @@
         <v>-135</v>
       </c>
       <c r="D2">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E2">
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -797,7 +1004,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -806,13 +1013,219 @@
         <v>-45</v>
       </c>
       <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4959C04F-C089-4289-9AA7-B87FF9B36F10}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>-90</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>-20</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D139DB8-6B4E-482B-A9C6-C5045EC5096E}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>-135</v>
+      </c>
+      <c r="D2">
+        <v>60</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>-45</v>
+      </c>
+      <c r="D3">
         <v>30</v>
       </c>
       <c r="E3">
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -820,10 +1233,414 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>-135</v>
+      </c>
+      <c r="D4">
+        <v>60</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>-45</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>-135</v>
+      </c>
+      <c r="D6">
+        <v>60</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>-45</v>
+      </c>
+      <c r="D7">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D310C4D-ACC7-4875-935C-22C25170EB0F}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>80</v>
+      </c>
+      <c r="E2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FAF2DEE-BB35-43FB-95A2-23207390B100}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>160</v>
+      </c>
+      <c r="E4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33649B24-74AC-4539-8031-350F2B274EE6}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>300</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{731C12B3-31EE-447B-AAAD-4F6B1A720D94}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added light display bad
</commit_message>
<xml_diff>
--- a/Choreography.xlsx
+++ b/Choreography.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc279616e9bf515a/Desktop/Robert/Uni/Fundamentals of Programming/Assignment V2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="326" documentId="8_{872808D0-E74D-4280-8616-FE908870EFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51037147-5BD4-493D-B371-40C275FB3597}"/>
+  <xr:revisionPtr revIDLastSave="366" documentId="8_{872808D0-E74D-4280-8616-FE908870EFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D72133AD-9C13-4D00-B8D4-779D491DCA3A}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6795" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{CA1F9D46-EE91-46A4-B57B-4EC92E55F95A}"/>
+    <workbookView xWindow="2544" yWindow="2220" windowWidth="17280" windowHeight="8880" firstSheet="2" activeTab="4" xr2:uid="{CA1F9D46-EE91-46A4-B57B-4EC92E55F95A}"/>
   </bookViews>
   <sheets>
     <sheet name="init" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,9 @@
     <sheet name="Light4" sheetId="8" r:id="rId5"/>
     <sheet name="machine1" sheetId="4" r:id="rId6"/>
     <sheet name="machine2" sheetId="7" r:id="rId7"/>
-    <sheet name="guitar" sheetId="6" r:id="rId8"/>
-    <sheet name="Key info" sheetId="5" r:id="rId9"/>
+    <sheet name="drum" sheetId="10" r:id="rId8"/>
+    <sheet name="guitar" sheetId="6" r:id="rId9"/>
+    <sheet name="Key info" sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="64">
   <si>
     <t>Type</t>
   </si>
@@ -230,6 +231,12 @@
   </si>
   <si>
     <t>yellow</t>
+  </si>
+  <si>
+    <t>drum</t>
+  </si>
+  <si>
+    <t>drum.png</t>
   </si>
 </sst>
 </file>
@@ -585,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E3453A-179F-4C57-94EA-DC41270CAC58}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -884,6 +891,109 @@
       </c>
       <c r="G16">
         <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17">
+        <v>200</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>150</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{731C12B3-31EE-447B-AAAD-4F6B1A720D94}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -947,7 +1057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB9F836-1785-4051-A1F8-E06C1617609E}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1043,7 +1153,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1153,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D139DB8-6B4E-482B-A9C6-C5045EC5096E}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1190,10 +1300,10 @@
         <v>34</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>-135</v>
+        <v>-100</v>
       </c>
       <c r="D2">
         <v>60</v>
@@ -1213,10 +1323,10 @@
         <v>34</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>-45</v>
+        <v>-160</v>
       </c>
       <c r="D3">
         <v>30</v>
@@ -1236,10 +1346,10 @@
         <v>34</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>-135</v>
+        <v>-100</v>
       </c>
       <c r="D4">
         <v>60</v>
@@ -1259,10 +1369,10 @@
         <v>34</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>-45</v>
+        <v>-160</v>
       </c>
       <c r="D5">
         <v>30</v>
@@ -1282,10 +1392,10 @@
         <v>34</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>-135</v>
+        <v>-100</v>
       </c>
       <c r="D6">
         <v>60</v>
@@ -1305,10 +1415,10 @@
         <v>34</v>
       </c>
       <c r="B7">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>-45</v>
+        <v>-160</v>
       </c>
       <c r="D7">
         <v>30</v>
@@ -1507,6 +1617,77 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5858ACEB-93DB-4020-90F5-1E5C60E569DE}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33649B24-74AC-4539-8031-350F2B274EE6}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1566,84 +1747,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{731C12B3-31EE-447B-AAAD-4F6B1A720D94}">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Commented and spaced everything Submittable Vesion
</commit_message>
<xml_diff>
--- a/Choreography.xlsx
+++ b/Choreography.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc279616e9bf515a/Desktop/Robert/Uni/Fundamentals of Programming/Assignment V2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="366" documentId="8_{872808D0-E74D-4280-8616-FE908870EFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D72133AD-9C13-4D00-B8D4-779D491DCA3A}"/>
+  <xr:revisionPtr revIDLastSave="368" documentId="8_{872808D0-E74D-4280-8616-FE908870EFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B29CD364-AE11-4FAF-B623-7651CF093076}"/>
   <bookViews>
-    <workbookView xWindow="2544" yWindow="2220" windowWidth="17280" windowHeight="8880" firstSheet="2" activeTab="4" xr2:uid="{CA1F9D46-EE91-46A4-B57B-4EC92E55F95A}"/>
+    <workbookView xWindow="-28920" yWindow="-6795" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="9" xr2:uid="{CA1F9D46-EE91-46A4-B57B-4EC92E55F95A}"/>
   </bookViews>
   <sheets>
     <sheet name="init" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="65">
   <si>
     <t>Type</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>drum.png</t>
+  </si>
+  <si>
+    <t>Only png image files supported</t>
   </si>
 </sst>
 </file>
@@ -925,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{731C12B3-31EE-447B-AAAD-4F6B1A720D94}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -949,6 +952,11 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1263,7 +1271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D139DB8-6B4E-482B-A9C6-C5045EC5096E}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>